<commit_message>
v2 of file editor and management
</commit_message>
<xml_diff>
--- a/core/media/uploads/sample_sheet.xlsx
+++ b/core/media/uploads/sample_sheet.xlsx
@@ -424,13 +424,15 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Sample Excel Data</t>
+          <t>Sample Excel Data test 2</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>12345</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>